<commit_message>
Enhance Level of Effort Excel formatting and update presales documents
Improved Level of Effort workbook formatting for better readability:
- Optimized column widths across all sheets (Scope Assumptions, Estimate Settings, LOE, Credits)
- Updated cover page to display "Level of Effort" as document type
- Relocated EO Sales Engineer note to bottom with red formatting
- Removed extra empty rows for cleaner presentation

Fixed solution briefing subtitle format:
- Updated solution-template to use proper provider + solution name format
- Aligned subtitle format with AWS IDP implementation pattern

Repository maintenance:
- Removed deprecated COST_CREDITS_GUIDANCE.md documentation
- Updated AWS IDP presales README with correct file references
- Regenerated all presales documents with latest templates

These changes improve document consistency and professional presentation across the EO Framework solution catalog.
</commit_message>
<xml_diff>
--- a/solution-template/sample-provider/sample-category/sample-solution/presales/level-of-effort-estimate.xlsx
+++ b/solution-template/sample-provider/sample-category/sample-solution/presales/level-of-effort-estimate.xlsx
@@ -13,8 +13,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Credits" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Scope Assumptions'!$A$2:$G$18</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Estimate Settings'!$A$2:$D$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Scope Assumptions'!$A$2:$G$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Estimate Settings'!$A$2:$D$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'LOE'!$A$2:$K$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Credits'!$A$2:$C$5</definedName>
   </definedNames>
@@ -29,7 +29,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="$#,##0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -133,6 +133,11 @@
       <name val="Calibri"/>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="00FF0000"/>
       <sz val="12"/>
     </font>
     <font>
@@ -420,49 +425,49 @@
     <xf numFmtId="165" fontId="2" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="18" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="18" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -839,7 +844,7 @@
     <row r="4" ht="25" customHeight="1">
       <c r="B4" s="15" t="inlineStr">
         <is>
-          <t>[Document Type]</t>
+          <t>Level of Effort</t>
         </is>
       </c>
     </row>
@@ -930,7 +935,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -941,11 +946,11 @@
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="30" customWidth="1" min="6" max="6"/>
-    <col width="40" customWidth="1" min="7" max="7"/>
+    <col width="33" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
+    <col width="32" customWidth="1" min="5" max="5"/>
+    <col width="39" customWidth="1" min="6" max="6"/>
+    <col width="44" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
@@ -1547,17 +1552,8 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="26" customHeight="1">
-      <c r="A18" s="40" t="inlineStr"/>
-      <c r="B18" s="41" t="inlineStr"/>
-      <c r="C18" s="39" t="inlineStr"/>
-      <c r="D18" s="41" t="inlineStr"/>
-      <c r="E18" s="41" t="inlineStr"/>
-      <c r="F18" s="41" t="inlineStr"/>
-      <c r="G18" s="41" t="inlineStr"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:G18"/>
+  <autoFilter ref="A2:G17"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
@@ -1571,7 +1567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1580,16 +1576,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="150" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="173" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
       <c r="A1" s="35" t="inlineStr">
         <is>
-          <t>ESTIMATE SETTINGS - EO Sales Engineer Updates Multipliers Based on Customer Scope</t>
+          <t>ESTIMATE SETTINGS</t>
         </is>
       </c>
     </row>
@@ -1795,16 +1791,18 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="26" customHeight="1">
-      <c r="A12" s="40" t="inlineStr"/>
-      <c r="B12" s="41" t="inlineStr"/>
-      <c r="C12" s="44" t="inlineStr"/>
-      <c r="D12" s="41" t="inlineStr"/>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" s="44" t="inlineStr">
+        <is>
+          <t>EO Sales Engineer Updates Multipliers Based on Customer Scope</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D12"/>
-  <mergeCells count="1">
+  <autoFilter ref="A2:D11"/>
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1825,10 +1823,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="58" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
@@ -3331,8 +3329,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
     <col width="100" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>

</xml_diff>